<commit_message>
Updated AK9943 board with improvements and worked master BOM
</commit_message>
<xml_diff>
--- a/Master BOM.xlsx
+++ b/Master BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhardin/Documents/EAGLE/projects/Dual-Mono-Amp-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11CAAE5C-A8E8-3843-9959-869D3B216D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8722AD9E-20C8-AB40-8A9D-B2EDCB3E0DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="3" xr2:uid="{462CCD63-FCCD-5945-8D12-2FB3BAFFC43C}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{AEF5911B-C563-5C46-BB8A-A64EB8BF7805}" name="AK4493-v1.64_23" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/AK4493-v1.64_23.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/AK4493-v1.64_23.txt" delimited="0">
       <textFields count="18">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -73,7 +73,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{79A58889-0CD9-AC4F-85EF-B2B123BED2FC}" name="AK4493-v1.64_231" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/AK4493-v1.64_23.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/AK4493-v1.64_23.txt" delimited="0">
       <textFields count="18">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -97,7 +97,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{FE31A6B3-AD0A-E748-A106-FDF9EAD1F767}" name="DAC_OutputStage 4 v4" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DAC_OutputStage 4 v4.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DAC_OutputStage 4 v4.txt" delimited="0">
       <textFields count="16">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -119,7 +119,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{6FECEB79-8614-D949-B900-8EE43514B9A2}" name="DAC_OutputStage 4 v41" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DAC_OutputStage 4 v4.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DAC_OutputStage 4 v4.txt" delimited="0">
       <textFields count="16">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -141,7 +141,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{900B489D-6811-674D-B0B3-EA6F25682FEA}" name="DualMonoPSU3" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DualMonoPSU3.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DualMonoPSU3.txt" delimited="0">
       <textFields count="16">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -163,7 +163,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{12C9A8E4-B1DC-A149-BBBD-471483880C93}" name="DualMonoPSU31" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DualMonoPSU3.txt" delimited="0">
+    <textPr firstRow="3" sourceFile="/Users/kevinhardin/Desktop/DualMonoPSU3.txt" delimited="0">
       <textFields count="16">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -1503,10 +1503,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1517,9 +1516,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1527,6 +1523,9 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1557,15 +1556,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DAC_OutputStage 4 v4" connectionId="4" xr16:uid="{487EA606-B959-5C4C-953E-908CECA512A8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DualMonoPSU3" connectionId="6" xr16:uid="{D6D2B277-857C-0942-90DA-5DB7135CCAE1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="AK4493-v1.64_23" connectionId="2" xr16:uid="{A503D8AF-E1E6-9140-A993-58AC352C14FF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DAC_OutputStage 4 v4" connectionId="4" xr16:uid="{487EA606-B959-5C4C-953E-908CECA512A8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5319,7 +5318,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5339,2225 +5338,2218 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="6"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="6"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="L15" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="19"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="6"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="6"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="6" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="6" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="6" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="6" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="L26" s="6" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="L27" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K28" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="L28" s="7" t="s">
+      <c r="L28" s="6" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="6" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="L30" s="6" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="6" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L32" s="6" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="L33" s="7" t="s">
+      <c r="L33" s="6" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="J34" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="L34" s="7" t="s">
+      <c r="L34" s="6" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="J35" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="K35" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="L35" s="6" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="J36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L36" s="7" t="s">
+      <c r="L36" s="6" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="K37" s="3" t="s">
+      <c r="K37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L37" s="7" t="s">
+      <c r="L37" s="6" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L38" s="7" t="s">
+      <c r="L38" s="6" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="6"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="K40" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L40" s="7" t="s">
+      <c r="L40" s="6" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="6"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I42" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J42" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="K42" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="L42" s="7" t="s">
+      <c r="L42" s="6" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="L43" s="7" t="s">
+      <c r="L43" s="6" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="6"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J45" s="3" t="s">
+      <c r="J45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="K45" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L45" s="7" t="s">
+      <c r="L45" s="6" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="J46" s="3" t="s">
+      <c r="J46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="K46" s="3"/>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="6"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G48" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="H48" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I48" s="9" t="s">
+      <c r="I48" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K48" s="9" t="s">
+      <c r="K48" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="L48" s="10" t="s">
+      <c r="L48" s="9" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
+    <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="15"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="21"/>
     </row>
     <row r="51" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="D51" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F51" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="H51" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I51" s="21" t="s">
+      <c r="I51" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J51" s="21" t="s">
+      <c r="J51" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="K51" s="21" t="s">
+      <c r="K51" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="L51" s="22" t="s">
+      <c r="L51" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17" t="s">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="19"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="15"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="L53" s="7" t="s">
+      <c r="L53" s="6" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="I54" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J54" s="3" t="s">
+      <c r="J54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="K54" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="L54" s="7" t="s">
+      <c r="L54" s="6" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="I55" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="J55" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="K55" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L55" s="7" t="s">
+      <c r="L55" s="6" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="I56" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J56" s="3" t="s">
+      <c r="J56" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="K56" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="L56" s="7" t="s">
+      <c r="L56" s="6" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H57" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I57" s="3" t="s">
+      <c r="I57" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J57" s="3" t="s">
+      <c r="J57" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="K57" s="4"/>
-      <c r="L57" s="6"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F58" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="I58" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="J58" s="3" t="s">
+      <c r="J58" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K58" s="4"/>
-      <c r="L58" s="6"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G59" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H59" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="I59" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J59" s="3" t="s">
+      <c r="J59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K59" s="3" t="s">
+      <c r="K59" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="L59" s="7" t="s">
+      <c r="L59" s="6" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G60" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="I60" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J60" s="3" t="s">
+      <c r="J60" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="K60" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="L60" s="7" t="s">
+      <c r="L60" s="6" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="I61" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J61" s="3" t="s">
+      <c r="J61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="L61" s="7" t="s">
+      <c r="L61" s="6" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="I62" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="J62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K62" s="3" t="s">
+      <c r="K62" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="L62" s="7" t="s">
+      <c r="L62" s="6" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H63" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I63" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J63" s="3" t="s">
+      <c r="J63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K63" s="3" t="s">
+      <c r="K63" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="L63" s="7" t="s">
+      <c r="L63" s="6" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I64" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="J64" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="K64" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="L64" s="7" t="s">
+      <c r="L64" s="6" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F65" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="I65" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J65" s="3" t="s">
+      <c r="J65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="K65" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="L65" s="7" t="s">
+      <c r="L65" s="6" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="6"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="I67" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J67" s="3" t="s">
+      <c r="J67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K67" s="4"/>
-      <c r="L67" s="6"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="5"/>
     </row>
     <row r="68" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E68" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="12"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>